<commit_message>
Fill cylinders now.  Needs HMI update
Signed-off-by: Doug Dmytryk <dougdmytryk@insight-analytical.com>
</commit_message>
<xml_diff>
--- a/Modbus Map - JP3 AUTOSAMPLER.xlsx
+++ b/Modbus Map - JP3 AUTOSAMPLER.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://insightvital.sharepoint.com/sites/Insight/Shared Documents/Service/JP3 AUTOSAMPLER/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dougd\Desktop\SAAS\JP3_AUTOSAMPLE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="40" documentId="13_ncr:1_{E764607E-D58B-47B8-8FBB-214375EFB747}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{C98EA9B5-5A94-4AC9-A3E0-C2DE6BF794AB}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50F4EFFE-89DB-49E1-B409-85BCD526E133}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{76F56F94-E428-4377-ACC8-5D902F9C5742}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{76F56F94-E428-4377-ACC8-5D902F9C5742}"/>
   </bookViews>
   <sheets>
     <sheet name="Autosampler PLC Modbus Map" sheetId="21" r:id="rId1"/>
@@ -1551,16 +1551,16 @@
     <xf numFmtId="0" fontId="25" fillId="0" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="61" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="61" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2062,28 +2062,28 @@
   </sheetPr>
   <dimension ref="A1:Q54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C55" sqref="C55"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.1328125" style="7" customWidth="1"/>
-    <col min="2" max="2" width="39.3984375" style="7" hidden="1" customWidth="1"/>
-    <col min="3" max="3" width="58.59765625" style="7" customWidth="1"/>
-    <col min="4" max="4" width="9.73046875" style="7" customWidth="1"/>
-    <col min="5" max="5" width="13.86328125" style="7" customWidth="1"/>
+    <col min="1" max="1" width="21.109375" style="7" customWidth="1"/>
+    <col min="2" max="2" width="39.44140625" style="7" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="58.5546875" style="7" customWidth="1"/>
+    <col min="4" max="4" width="9.77734375" style="7" customWidth="1"/>
+    <col min="5" max="5" width="13.88671875" style="7" customWidth="1"/>
     <col min="6" max="6" width="24" style="40" customWidth="1"/>
-    <col min="7" max="7" width="7.265625" style="7" customWidth="1"/>
-    <col min="8" max="13" width="11.73046875" style="7" customWidth="1"/>
-    <col min="14" max="14" width="15.73046875" style="7" customWidth="1"/>
+    <col min="7" max="7" width="7.21875" style="7" customWidth="1"/>
+    <col min="8" max="13" width="11.77734375" style="7" customWidth="1"/>
+    <col min="14" max="14" width="15.77734375" style="7" customWidth="1"/>
     <col min="15" max="15" width="14" style="7" customWidth="1"/>
-    <col min="16" max="16" width="53.73046875" style="7" customWidth="1"/>
-    <col min="17" max="17" width="46.1328125" style="7" customWidth="1"/>
-    <col min="18" max="16384" width="9.1328125" style="7"/>
+    <col min="16" max="16" width="53.77734375" style="7" customWidth="1"/>
+    <col min="17" max="17" width="46.109375" style="7" customWidth="1"/>
+    <col min="18" max="16384" width="9.109375" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:17" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="61" t="s">
         <v>0</v>
       </c>
@@ -2104,7 +2104,7 @@
       <c r="P1" s="51"/>
       <c r="Q1" s="51"/>
     </row>
-    <row r="2" spans="1:17" ht="66" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:17" ht="66" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
         <v>1</v>
       </c>
@@ -2157,28 +2157,28 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:17" s="4" customFormat="1" ht="49.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="64" t="s">
+    <row r="3" spans="1:17" s="4" customFormat="1" ht="49.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="62" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="65"/>
-      <c r="C3" s="65"/>
-      <c r="D3" s="65"/>
-      <c r="E3" s="65"/>
-      <c r="F3" s="65"/>
-      <c r="G3" s="65"/>
-      <c r="H3" s="65"/>
-      <c r="I3" s="65"/>
-      <c r="J3" s="65"/>
-      <c r="K3" s="65"/>
-      <c r="L3" s="65"/>
-      <c r="M3" s="65"/>
-      <c r="N3" s="65"/>
-      <c r="O3" s="65"/>
-      <c r="P3" s="65"/>
+      <c r="B3" s="63"/>
+      <c r="C3" s="63"/>
+      <c r="D3" s="63"/>
+      <c r="E3" s="63"/>
+      <c r="F3" s="63"/>
+      <c r="G3" s="63"/>
+      <c r="H3" s="63"/>
+      <c r="I3" s="63"/>
+      <c r="J3" s="63"/>
+      <c r="K3" s="63"/>
+      <c r="L3" s="63"/>
+      <c r="M3" s="63"/>
+      <c r="N3" s="63"/>
+      <c r="O3" s="63"/>
+      <c r="P3" s="63"/>
       <c r="Q3" s="52"/>
     </row>
-    <row r="4" spans="1:17" ht="66" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:17" ht="66" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="8" t="s">
         <v>1</v>
       </c>
@@ -2231,7 +2231,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:17" s="4" customFormat="1" ht="34.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:17" s="4" customFormat="1" ht="34.200000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="53"/>
       <c r="B5" s="12" t="s">
         <v>19</v>
@@ -2278,7 +2278,7 @@
       <c r="P5" s="3"/>
       <c r="Q5" s="38"/>
     </row>
-    <row r="6" spans="1:17" s="4" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:17" s="4" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="14"/>
       <c r="B6" s="15" t="s">
         <v>24</v>
@@ -2325,7 +2325,7 @@
       <c r="P6" s="17"/>
       <c r="Q6" s="57"/>
     </row>
-    <row r="7" spans="1:17" s="4" customFormat="1" ht="25.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:17" s="4" customFormat="1" ht="25.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="18"/>
       <c r="B7" s="12" t="s">
         <v>28</v>
@@ -2372,7 +2372,7 @@
       <c r="P7" s="3"/>
       <c r="Q7" s="38"/>
     </row>
-    <row r="8" spans="1:17" s="4" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:17" s="4" customFormat="1" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="53"/>
       <c r="B8" s="12" t="s">
         <v>31</v>
@@ -2416,12 +2416,12 @@
       <c r="O8" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="P8" s="62" t="s">
+      <c r="P8" s="64" t="s">
         <v>33</v>
       </c>
       <c r="Q8" s="38"/>
     </row>
-    <row r="9" spans="1:17" s="4" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:17" s="4" customFormat="1" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="53"/>
       <c r="B9" s="12" t="s">
         <v>34</v>
@@ -2465,10 +2465,10 @@
       <c r="O9" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="P9" s="63"/>
+      <c r="P9" s="65"/>
       <c r="Q9" s="38"/>
     </row>
-    <row r="10" spans="1:17" s="4" customFormat="1" ht="25.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:17" s="4" customFormat="1" ht="25.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="18"/>
       <c r="B10" s="12"/>
       <c r="C10" s="12" t="s">
@@ -2515,7 +2515,7 @@
       </c>
       <c r="Q10" s="19"/>
     </row>
-    <row r="11" spans="1:17" s="4" customFormat="1" ht="25.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:17" s="4" customFormat="1" ht="25.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="18"/>
       <c r="B11" s="12"/>
       <c r="C11" s="12" t="s">
@@ -2562,7 +2562,7 @@
       </c>
       <c r="Q11" s="19"/>
     </row>
-    <row r="12" spans="1:17" s="4" customFormat="1" ht="25.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:17" s="4" customFormat="1" ht="25.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="18"/>
       <c r="B12" s="12"/>
       <c r="C12" s="12" t="s">
@@ -2609,7 +2609,7 @@
       </c>
       <c r="Q12" s="19"/>
     </row>
-    <row r="13" spans="1:17" s="4" customFormat="1" ht="25.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:17" s="4" customFormat="1" ht="25.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="18"/>
       <c r="B13" s="12"/>
       <c r="C13" s="12" t="s">
@@ -2656,7 +2656,7 @@
       </c>
       <c r="Q13" s="19"/>
     </row>
-    <row r="14" spans="1:17" s="4" customFormat="1" ht="25.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:17" s="4" customFormat="1" ht="25.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="22"/>
       <c r="B14" s="23"/>
       <c r="C14" s="23" t="s">
@@ -2703,7 +2703,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="15" spans="1:17" s="4" customFormat="1" ht="25.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:17" s="4" customFormat="1" ht="25.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="18"/>
       <c r="B15" s="12"/>
       <c r="C15" s="12" t="s">
@@ -2750,7 +2750,7 @@
       </c>
       <c r="Q15" s="19"/>
     </row>
-    <row r="16" spans="1:17" s="4" customFormat="1" ht="25.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:17" s="4" customFormat="1" ht="25.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="18"/>
       <c r="B16" s="12"/>
       <c r="C16" s="12" t="s">
@@ -2797,7 +2797,7 @@
       </c>
       <c r="Q16" s="19"/>
     </row>
-    <row r="17" spans="1:17" s="4" customFormat="1" ht="25.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:17" s="4" customFormat="1" ht="25.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="18"/>
       <c r="B17" s="12"/>
       <c r="C17" s="12" t="s">
@@ -2846,7 +2846,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="18" spans="1:17" s="4" customFormat="1" ht="25.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:17" s="4" customFormat="1" ht="25.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="18"/>
       <c r="B18" s="12"/>
       <c r="C18" s="12" t="s">
@@ -2893,7 +2893,7 @@
       </c>
       <c r="Q18" s="19"/>
     </row>
-    <row r="19" spans="1:17" s="4" customFormat="1" ht="25.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:17" s="4" customFormat="1" ht="25.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="18"/>
       <c r="B19" s="12"/>
       <c r="C19" s="12" t="s">
@@ -2942,7 +2942,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="20" spans="1:17" s="4" customFormat="1" ht="25.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:17" s="4" customFormat="1" ht="25.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="22"/>
       <c r="B20" s="23"/>
       <c r="C20" s="23" t="s">
@@ -2991,7 +2991,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="21" spans="1:17" s="4" customFormat="1" ht="25.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:17" s="4" customFormat="1" ht="25.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="14"/>
       <c r="B21" s="15"/>
       <c r="C21" s="30" t="s">
@@ -3038,7 +3038,7 @@
       </c>
       <c r="Q21" s="34"/>
     </row>
-    <row r="22" spans="1:17" s="4" customFormat="1" ht="25.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:17" s="4" customFormat="1" ht="25.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="18"/>
       <c r="B22" s="12"/>
       <c r="C22" s="35" t="s">
@@ -3085,7 +3085,7 @@
       </c>
       <c r="Q22" s="19"/>
     </row>
-    <row r="23" spans="1:17" s="4" customFormat="1" ht="25.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:17" s="4" customFormat="1" ht="25.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="22"/>
       <c r="B23" s="23"/>
       <c r="C23" s="36" t="s">
@@ -3132,7 +3132,7 @@
       </c>
       <c r="Q23" s="28"/>
     </row>
-    <row r="24" spans="1:17" s="4" customFormat="1" ht="25.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:17" s="4" customFormat="1" ht="25.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="18"/>
       <c r="B24" s="12"/>
       <c r="C24" s="35" t="s">
@@ -3179,7 +3179,7 @@
       </c>
       <c r="Q24" s="19"/>
     </row>
-    <row r="25" spans="1:17" s="4" customFormat="1" ht="25.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:17" s="4" customFormat="1" ht="25.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="18"/>
       <c r="B25" s="12"/>
       <c r="C25" s="35" t="s">
@@ -3226,7 +3226,7 @@
       </c>
       <c r="Q25" s="19"/>
     </row>
-    <row r="26" spans="1:17" s="4" customFormat="1" ht="25.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:17" s="4" customFormat="1" ht="25.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="18"/>
       <c r="B26" s="12"/>
       <c r="C26" s="35" t="s">
@@ -3273,7 +3273,7 @@
       </c>
       <c r="Q26" s="19"/>
     </row>
-    <row r="27" spans="1:17" s="4" customFormat="1" ht="25.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:17" s="4" customFormat="1" ht="25.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="14"/>
       <c r="B27" s="15"/>
       <c r="C27" s="30" t="s">
@@ -3320,7 +3320,7 @@
       </c>
       <c r="Q27" s="34"/>
     </row>
-    <row r="28" spans="1:17" s="4" customFormat="1" ht="25.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:17" s="4" customFormat="1" ht="25.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="18"/>
       <c r="B28" s="12"/>
       <c r="C28" s="35" t="s">
@@ -3367,7 +3367,7 @@
       </c>
       <c r="Q28" s="19"/>
     </row>
-    <row r="29" spans="1:17" s="4" customFormat="1" ht="25.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:17" s="4" customFormat="1" ht="25.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="22"/>
       <c r="B29" s="23"/>
       <c r="C29" s="36" t="s">
@@ -3414,7 +3414,7 @@
       </c>
       <c r="Q29" s="28"/>
     </row>
-    <row r="30" spans="1:17" s="4" customFormat="1" ht="25.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:17" s="4" customFormat="1" ht="25.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="18"/>
       <c r="B30" s="12"/>
       <c r="C30" s="35" t="s">
@@ -3461,7 +3461,7 @@
       </c>
       <c r="Q30" s="19"/>
     </row>
-    <row r="31" spans="1:17" s="4" customFormat="1" ht="25.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:17" s="4" customFormat="1" ht="25.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="18"/>
       <c r="B31" s="12"/>
       <c r="C31" s="35" t="s">
@@ -3508,7 +3508,7 @@
       </c>
       <c r="Q31" s="19"/>
     </row>
-    <row r="32" spans="1:17" s="4" customFormat="1" ht="25.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:17" s="4" customFormat="1" ht="25.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="22"/>
       <c r="B32" s="23"/>
       <c r="C32" s="36" t="s">
@@ -3555,7 +3555,7 @@
       </c>
       <c r="Q32" s="28"/>
     </row>
-    <row r="33" spans="1:17" s="4" customFormat="1" ht="25.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:17" s="4" customFormat="1" ht="25.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="22"/>
       <c r="B33" s="23"/>
       <c r="C33" s="36" t="s">
@@ -3602,11 +3602,11 @@
       </c>
       <c r="Q33" s="28"/>
     </row>
-    <row r="34" spans="1:17" s="4" customFormat="1" ht="25.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:17" s="4" customFormat="1" ht="25.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="22"/>
       <c r="B34" s="23"/>
       <c r="C34" s="36" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D34" s="24" t="s">
         <v>21</v>
@@ -3649,7 +3649,7 @@
       </c>
       <c r="Q34" s="28"/>
     </row>
-    <row r="35" spans="1:17" s="4" customFormat="1" ht="25.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:17" s="4" customFormat="1" ht="25.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="22"/>
       <c r="B35" s="23"/>
       <c r="C35" s="36" t="s">
@@ -3696,7 +3696,7 @@
       </c>
       <c r="Q35" s="28"/>
     </row>
-    <row r="36" spans="1:17" s="39" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:17" s="39" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="42"/>
       <c r="B36" s="43" t="s">
         <v>80</v>
@@ -3745,7 +3745,7 @@
       </c>
       <c r="Q36" s="46"/>
     </row>
-    <row r="37" spans="1:17" s="39" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:17" s="39" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="42"/>
       <c r="B37" s="43" t="s">
         <v>80</v>
@@ -3794,7 +3794,7 @@
       </c>
       <c r="Q37" s="46"/>
     </row>
-    <row r="38" spans="1:17" s="39" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:17" s="39" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="18"/>
       <c r="B38" s="12" t="s">
         <v>87</v>
@@ -3843,7 +3843,7 @@
       </c>
       <c r="Q38" s="38"/>
     </row>
-    <row r="39" spans="1:17" s="39" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:17" s="39" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="18"/>
       <c r="B39" s="12" t="s">
         <v>90</v>
@@ -3892,7 +3892,7 @@
       </c>
       <c r="Q39" s="38"/>
     </row>
-    <row r="40" spans="1:17" s="39" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:17" s="39" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="18"/>
       <c r="B40" s="12" t="s">
         <v>93</v>
@@ -3941,7 +3941,7 @@
       </c>
       <c r="Q40" s="38"/>
     </row>
-    <row r="41" spans="1:17" s="39" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:17" s="39" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="18"/>
       <c r="B41" s="12" t="s">
         <v>96</v>
@@ -3990,7 +3990,7 @@
       </c>
       <c r="Q41" s="38"/>
     </row>
-    <row r="42" spans="1:17" s="39" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:17" s="39" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="18"/>
       <c r="B42" s="12" t="s">
         <v>99</v>
@@ -4039,7 +4039,7 @@
       </c>
       <c r="Q42" s="38"/>
     </row>
-    <row r="43" spans="1:17" s="4" customFormat="1" ht="25.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:17" s="4" customFormat="1" ht="25.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="18"/>
       <c r="B43" s="12" t="s">
         <v>102</v>
@@ -4086,7 +4086,7 @@
       <c r="P43" s="3"/>
       <c r="Q43" s="38"/>
     </row>
-    <row r="44" spans="1:17" s="4" customFormat="1" ht="25.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:17" s="4" customFormat="1" ht="25.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="18"/>
       <c r="B44" s="12" t="s">
         <v>104</v>
@@ -4133,7 +4133,7 @@
       <c r="P44" s="3"/>
       <c r="Q44" s="38"/>
     </row>
-    <row r="45" spans="1:17" s="4" customFormat="1" ht="25.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:17" s="4" customFormat="1" ht="25.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="18"/>
       <c r="B45" s="12" t="s">
         <v>106</v>
@@ -4180,7 +4180,7 @@
       <c r="P45" s="3"/>
       <c r="Q45" s="38"/>
     </row>
-    <row r="46" spans="1:17" s="4" customFormat="1" ht="25.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:17" s="4" customFormat="1" ht="25.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="53"/>
       <c r="B46" s="59" t="s">
         <v>108</v>
@@ -4227,7 +4227,7 @@
       <c r="P46" s="3"/>
       <c r="Q46" s="38"/>
     </row>
-    <row r="47" spans="1:17" s="4" customFormat="1" ht="25.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:17" s="4" customFormat="1" ht="25.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="53"/>
       <c r="B47" s="59" t="s">
         <v>111</v>
@@ -4274,7 +4274,7 @@
       <c r="P47" s="3"/>
       <c r="Q47" s="38"/>
     </row>
-    <row r="48" spans="1:17" s="4" customFormat="1" ht="25.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:17" s="4" customFormat="1" ht="25.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="53"/>
       <c r="B48" s="59" t="s">
         <v>113</v>
@@ -4321,7 +4321,7 @@
       <c r="P48" s="3"/>
       <c r="Q48" s="38"/>
     </row>
-    <row r="49" spans="1:17" s="4" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:17" s="4" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="18"/>
       <c r="B49" s="59" t="s">
         <v>115</v>
@@ -4368,7 +4368,7 @@
       <c r="P49" s="3"/>
       <c r="Q49" s="38"/>
     </row>
-    <row r="50" spans="1:17" s="4" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:17" s="4" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="18"/>
       <c r="B50" s="59" t="s">
         <v>117</v>
@@ -4415,7 +4415,7 @@
       <c r="P50" s="3"/>
       <c r="Q50" s="38"/>
     </row>
-    <row r="51" spans="1:17" s="4" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:17" s="4" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="53"/>
       <c r="B51" s="59" t="s">
         <v>119</v>
@@ -4462,7 +4462,7 @@
       <c r="P51" s="60"/>
       <c r="Q51" s="19"/>
     </row>
-    <row r="52" spans="1:17" s="4" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:17" s="4" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="53"/>
       <c r="B52" s="59" t="s">
         <v>121</v>
@@ -4509,7 +4509,7 @@
       <c r="P52" s="60"/>
       <c r="Q52" s="19"/>
     </row>
-    <row r="53" spans="1:17" s="4" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:17" s="4" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="53"/>
       <c r="B53" s="59" t="s">
         <v>123</v>
@@ -4556,13 +4556,13 @@
       <c r="P53" s="60"/>
       <c r="Q53" s="19"/>
     </row>
-    <row r="54" spans="1:17" s="4" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:17" s="4" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="53"/>
       <c r="B54" s="59" t="s">
         <v>123</v>
       </c>
       <c r="C54" s="13" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="D54" s="37" t="s">
         <v>26</v>
@@ -4626,6 +4626,21 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A9E048A78312A94897F0E6646B12AFBF" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="bd08b2505fc4b2d71d7f81a4b53a834e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="b8b857fa-ab8c-46db-8ae6-f4c6b17fc121" xmlns:ns3="27204c16-4a37-455d-9af4-3dab56a7ac7c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="abb89873d455ab885c287f7d103a602b" ns2:_="" ns3:_="">
     <xsd:import namespace="b8b857fa-ab8c-46db-8ae6-f4c6b17fc121"/>
@@ -4842,21 +4857,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{32566D75-CE0F-402B-9272-B6CBF9A57ECC}">
   <ds:schemaRefs>
@@ -4866,20 +4866,9 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3E0609E9-9BEB-4461-B97D-B5E7A06127C0}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{22CD16C8-4CA8-4223-86A7-0732D792A0E9}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="b8b857fa-ab8c-46db-8ae6-f4c6b17fc121"/>
-    <ds:schemaRef ds:uri="27204c16-4a37-455d-9af4-3dab56a7ac7c"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -4902,9 +4891,20 @@
 </file>
 
 <file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{22CD16C8-4CA8-4223-86A7-0732D792A0E9}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3E0609E9-9BEB-4461-B97D-B5E7A06127C0}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="b8b857fa-ab8c-46db-8ae6-f4c6b17fc121"/>
+    <ds:schemaRef ds:uri="27204c16-4a37-455d-9af4-3dab56a7ac7c"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>